<commit_message>
Recuperação de informação TP3
</commit_message>
<xml_diff>
--- a/Recuperação de Informação/ES05.xlsx
+++ b/Recuperação de Informação/ES05.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zorak\Documents\5Periodo\Recuperação de Informação\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C621B11D-9089-4199-B139-E510A54478D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F66CC96-C579-4AD7-AF1E-A13E34258BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="612" windowWidth="23256" windowHeight="12456" xr2:uid="{DB51CADD-8B23-45DF-ADA5-8881F384A387}"/>
+    <workbookView xWindow="-108" yWindow="612" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{DB51CADD-8B23-45DF-ADA5-8881F384A387}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="63">
   <si>
     <t>q1</t>
   </si>
@@ -380,7 +380,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -406,10 +406,22 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -421,22 +433,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -794,6 +797,7 @@
         <c:axId val="1529559615"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1262,6 +1266,7 @@
         <c:axId val="1644738015"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2936,7 +2941,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8DDB83-FAC6-4291-BECF-10D3138C5D21}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="D1" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
@@ -2948,34 +2953,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="18"/>
+      <c r="G2" s="14"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
@@ -3008,7 +3013,7 @@
       <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="9" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="6" t="s">
@@ -3033,7 +3038,7 @@
       <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="9" t="s">
         <v>26</v>
       </c>
       <c r="C5" s="6" t="s">
@@ -3064,7 +3069,7 @@
       <c r="C6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="9" t="s">
         <v>29</v>
       </c>
       <c r="E6" s="6" t="s">
@@ -3089,13 +3094,13 @@
       <c r="C7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="9" t="s">
         <v>25</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="9" t="s">
         <v>29</v>
       </c>
       <c r="G7" s="6" t="s">
@@ -3108,7 +3113,7 @@
       <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="9" t="s">
         <v>29</v>
       </c>
       <c r="C8" s="6" t="s">
@@ -3120,7 +3125,7 @@
       <c r="E8" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="9" t="s">
         <v>25</v>
       </c>
       <c r="G8" s="6" t="s">
@@ -3263,10 +3268,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA7B30F4-C5E6-4AEA-916D-14F03ACF7C42}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9:G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3278,32 +3283,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="8"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="18"/>
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16" t="s">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="16"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -3326,83 +3331,212 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="19">
+      <c r="B4" s="11">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="11">
         <f>1/1</f>
         <v>1</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="11">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="11">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="11">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="11">
         <f>1/4</f>
         <v>0.25</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="19">
+      <c r="B5" s="11">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="11">
         <f>2/2</f>
         <v>1</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="11">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="11">
         <f>2/4</f>
         <v>0.5</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="11">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="11">
         <f>2/5</f>
         <v>0.4</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="19">
+      <c r="B6" s="11">
         <f>3/3</f>
         <v>1</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="11">
         <f>3/5</f>
         <v>0.6</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="11">
         <f>3/3</f>
         <v>1</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="11">
         <v>0</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="11">
         <f>3/3</f>
         <v>1</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="11">
         <v>0</v>
       </c>
     </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="18"/>
+      <c r="D9" s="18"/>
+      <c r="E9" s="18"/>
+      <c r="F9" s="18"/>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="18"/>
+      <c r="B10" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="12"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>61</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B12" s="11">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C12" s="11">
+        <f>1/1</f>
+        <v>1</v>
+      </c>
+      <c r="D12" s="11">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E12" s="11">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="F12" s="11">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="G12" s="11">
+        <f>1/4</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B13" s="11">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C13" s="11">
+        <f>2/2</f>
+        <v>1</v>
+      </c>
+      <c r="D13" s="11">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E13" s="11">
+        <f>2/4</f>
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="11">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="G13" s="11">
+        <f>2/5</f>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B14" s="11">
+        <f>3/3</f>
+        <v>1</v>
+      </c>
+      <c r="C14" s="11">
+        <f>3/5</f>
+        <v>0.6</v>
+      </c>
+      <c r="D14" s="11">
+        <f>3/3</f>
+        <v>1</v>
+      </c>
+      <c r="E14" s="11">
+        <v>0</v>
+      </c>
+      <c r="F14" s="11">
+        <f>3/3</f>
+        <v>1</v>
+      </c>
+      <c r="G14" s="11">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="10">
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="B9:G9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="F10:G10"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:C2"/>
@@ -3430,32 +3564,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="8" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="8"/>
+      <c r="C2" s="18"/>
       <c r="D2" s="5"/>
       <c r="E2" s="5"/>
-      <c r="F2" s="9" t="s">
+      <c r="F2" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="10"/>
+      <c r="G2" s="20"/>
       <c r="H2" s="2"/>
       <c r="I2" s="2"/>
     </row>
@@ -3550,7 +3684,7 @@
       <c r="E6" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="10" t="s">
         <v>28</v>
       </c>
       <c r="G6" s="6" t="s">
@@ -3594,7 +3728,7 @@
       <c r="C8" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="D8" s="15" t="s">
+      <c r="D8" s="10" t="s">
         <v>28</v>
       </c>
       <c r="E8" s="6" t="s">
@@ -3650,7 +3784,7 @@
       <c r="E10" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="10" t="s">
         <v>26</v>
       </c>
       <c r="G10" s="6" t="s">
@@ -3669,7 +3803,7 @@
       <c r="C11" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="D11" s="15" t="s">
+      <c r="D11" s="10" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="6" t="s">
@@ -3777,32 +3911,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="12"/>
-      <c r="B2" s="16" t="s">
+      <c r="A2" s="16"/>
+      <c r="B2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="17" t="s">
+      <c r="C2" s="12"/>
+      <c r="D2" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="18"/>
-      <c r="F2" s="17" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="18"/>
+      <c r="G2" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="4" t="s">
@@ -3825,78 +3959,78 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B4" s="19">
+      <c r="B4" s="11">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="C4" s="19">
+      <c r="C4" s="11">
         <f>1/2</f>
         <v>0.5</v>
       </c>
-      <c r="D4" s="19">
+      <c r="D4" s="11">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E4" s="19">
+      <c r="E4" s="11">
         <f>1/5</f>
         <v>0.2</v>
       </c>
-      <c r="F4" s="19">
+      <c r="F4" s="11">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G4" s="19">
+      <c r="G4" s="11">
         <f>1/3</f>
         <v>0.33333333333333331</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B5" s="19">
+      <c r="B5" s="11">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="C5" s="19">
+      <c r="C5" s="11">
         <f>2/4</f>
         <v>0.5</v>
       </c>
-      <c r="D5" s="19">
+      <c r="D5" s="11">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="E5" s="19">
+      <c r="E5" s="11">
         <f>1/8</f>
         <v>0.125</v>
       </c>
-      <c r="F5" s="19">
+      <c r="F5" s="11">
         <f>2/3</f>
         <v>0.66666666666666663</v>
       </c>
-      <c r="G5" s="19">
+      <c r="G5" s="11">
         <f>2/7</f>
         <v>0.2857142857142857</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="B6" s="19">
+      <c r="B6" s="11">
         <f>3/3</f>
         <v>1</v>
       </c>
-      <c r="C6" s="19">
+      <c r="C6" s="11">
         <f>3/10</f>
         <v>0.3</v>
       </c>
-      <c r="D6" s="19">
+      <c r="D6" s="11">
         <f>3/3</f>
         <v>1</v>
       </c>
-      <c r="E6" s="19">
+      <c r="E6" s="11">
         <v>0</v>
       </c>
-      <c r="F6" s="19">
+      <c r="F6" s="11">
         <f>3/3</f>
         <v>1</v>
       </c>
-      <c r="G6" s="19">
+      <c r="G6" s="11">
         <v>0</v>
       </c>
     </row>

</xml_diff>